<commit_message>
Day 06 - Tạo đường dẫn đến các page sử dụng navigo
</commit_message>
<xml_diff>
--- a/diem_danh_giay_10_05_23_08_00_51.xlsx
+++ b/diem_danh_giay_10_05_23_08_00_51.xlsx
@@ -409,9 +409,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="dd\-mmm"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
@@ -443,13 +443,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -463,9 +456,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -479,33 +486,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -526,7 +511,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -534,7 +519,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -549,33 +549,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -587,7 +571,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -614,7 +614,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -626,13 +626,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -644,13 +650,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -662,43 +722,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -710,61 +746,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -777,6 +759,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -829,6 +829,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -851,36 +866,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -908,151 +893,166 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1472,8 +1472,8 @@
   <sheetPr/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1482,7 +1482,8 @@
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
     <col min="4" max="4" width="20.109375" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="5" max="5" width="2.453125" customWidth="1"/>
+    <col min="6" max="6" width="2.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -1618,8 +1619,12 @@
       <c r="F5" s="12">
         <v>45063</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="G5" s="12">
+        <v>45068</v>
+      </c>
+      <c r="H5" s="12">
+        <v>45070</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -1656,8 +1661,12 @@
       <c r="F6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -1694,8 +1703,12 @@
       <c r="F7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -1732,8 +1745,12 @@
       <c r="F8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -1770,8 +1787,12 @@
       <c r="F9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1808,8 +1829,12 @@
       <c r="F10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -1846,8 +1871,12 @@
       <c r="F11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="G11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1884,8 +1913,12 @@
       <c r="F12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -1922,8 +1955,12 @@
       <c r="F13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1960,8 +1997,12 @@
       <c r="F14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="G14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1998,8 +2039,12 @@
       <c r="F15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="G15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -2036,8 +2081,12 @@
       <c r="F16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="G16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -2074,8 +2123,12 @@
       <c r="F17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="G17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -2112,8 +2165,12 @@
       <c r="F18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="G18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -2150,8 +2207,12 @@
       <c r="F19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="G19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -2188,8 +2249,12 @@
       <c r="F20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="G20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -2226,8 +2291,12 @@
       <c r="F21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="G21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -2264,8 +2333,12 @@
       <c r="F22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
+      <c r="G22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -2302,8 +2375,12 @@
       <c r="F23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
+      <c r="G23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -2340,8 +2417,12 @@
       <c r="F24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
+      <c r="G24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -2378,8 +2459,12 @@
       <c r="F25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="G25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -2416,8 +2501,12 @@
       <c r="F26" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
+      <c r="G26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -2454,8 +2543,12 @@
       <c r="F27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
+      <c r="G27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -2492,8 +2585,12 @@
       <c r="F28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
+      <c r="G28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -2530,8 +2627,12 @@
       <c r="F29" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
+      <c r="G29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -2568,8 +2669,12 @@
       <c r="F30" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
+      <c r="G30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
@@ -2606,8 +2711,12 @@
       <c r="F31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
+      <c r="G31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
@@ -2644,8 +2753,12 @@
       <c r="F32" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
+      <c r="G32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -2682,8 +2795,12 @@
       <c r="F33" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
+      <c r="G33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -2720,8 +2837,12 @@
       <c r="F34" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
+      <c r="G34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
@@ -2758,8 +2879,12 @@
       <c r="F35" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
+      <c r="G35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -2796,8 +2921,12 @@
       <c r="F36" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
+      <c r="G36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
@@ -2834,8 +2963,12 @@
       <c r="F37" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
+      <c r="G37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
@@ -2872,8 +3005,12 @@
       <c r="F38" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
+      <c r="G38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
@@ -2910,8 +3047,12 @@
       <c r="F39" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
+      <c r="G39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
@@ -2948,8 +3089,12 @@
       <c r="F40" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
+      <c r="G40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
@@ -2986,8 +3131,12 @@
       <c r="F41" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
+      <c r="G41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
@@ -3024,8 +3173,12 @@
       <c r="F42" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
+      <c r="G42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>

</xml_diff>

<commit_message>
Day 09 - fetch api + management page
</commit_message>
<xml_diff>
--- a/diem_danh_giay_10_05_23_08_00_51.xlsx
+++ b/diem_danh_giay_10_05_23_08_00_51.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowHeight="18800"/>
+    <workbookView windowWidth="25600" windowHeight="10800"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -408,11 +408,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="dd\-mmm"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="dd\-mmm"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -452,20 +452,51 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -478,19 +509,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -503,15 +534,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -532,9 +555,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -548,46 +577,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -608,7 +608,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -620,13 +644,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -638,13 +704,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -656,55 +758,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -716,73 +776,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -807,50 +807,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -888,8 +844,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -908,151 +864,195 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1472,8 +1472,8 @@
   <sheetPr/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1484,6 +1484,8 @@
     <col min="4" max="4" width="20.109375" customWidth="1"/>
     <col min="5" max="5" width="2.453125" customWidth="1"/>
     <col min="6" max="6" width="2.75" customWidth="1"/>
+    <col min="7" max="7" width="1.953125" customWidth="1"/>
+    <col min="8" max="8" width="2.234375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -1625,7 +1627,9 @@
       <c r="H5" s="12">
         <v>45070</v>
       </c>
-      <c r="I5" s="1"/>
+      <c r="I5" s="12">
+        <v>45072</v>
+      </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -1667,7 +1671,9 @@
       <c r="H6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="1"/>
+      <c r="I6" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -1709,7 +1715,9 @@
       <c r="H7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -1751,7 +1759,9 @@
       <c r="H8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -1793,7 +1803,9 @@
       <c r="H9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="1"/>
+      <c r="I9" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -1835,7 +1847,9 @@
       <c r="H10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="1"/>
+      <c r="I10" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -1877,7 +1891,9 @@
       <c r="H11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="1"/>
+      <c r="I11" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -1919,7 +1935,9 @@
       <c r="H12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="1"/>
+      <c r="I12" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -1961,7 +1979,9 @@
       <c r="H13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="1"/>
+      <c r="I13" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -2003,7 +2023,9 @@
       <c r="H14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="1"/>
+      <c r="I14" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -2045,7 +2067,9 @@
       <c r="H15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="1"/>
+      <c r="I15" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -2087,7 +2111,9 @@
       <c r="H16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I16" s="1"/>
+      <c r="I16" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -2129,7 +2155,9 @@
       <c r="H17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="1"/>
+      <c r="I17" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -2171,7 +2199,9 @@
       <c r="H18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I18" s="1"/>
+      <c r="I18" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -2213,7 +2243,9 @@
       <c r="H19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I19" s="1"/>
+      <c r="I19" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -2255,7 +2287,9 @@
       <c r="H20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I20" s="1"/>
+      <c r="I20" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -2297,7 +2331,9 @@
       <c r="H21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="1"/>
+      <c r="I21" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -2339,7 +2375,9 @@
       <c r="H22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I22" s="1"/>
+      <c r="I22" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -2381,7 +2419,9 @@
       <c r="H23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I23" s="1"/>
+      <c r="I23" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -2423,7 +2463,9 @@
       <c r="H24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I24" s="1"/>
+      <c r="I24" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -2465,7 +2507,9 @@
       <c r="H25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I25" s="1"/>
+      <c r="I25" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -2507,7 +2551,9 @@
       <c r="H26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I26" s="1"/>
+      <c r="I26" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -2549,7 +2595,9 @@
       <c r="H27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I27" s="1"/>
+      <c r="I27" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -2591,7 +2639,9 @@
       <c r="H28" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I28" s="1"/>
+      <c r="I28" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -2633,7 +2683,9 @@
       <c r="H29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I29" s="1"/>
+      <c r="I29" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
@@ -2675,7 +2727,9 @@
       <c r="H30" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I30" s="1"/>
+      <c r="I30" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
@@ -2717,7 +2771,9 @@
       <c r="H31" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I31" s="1"/>
+      <c r="I31" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -2759,7 +2815,9 @@
       <c r="H32" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I32" s="1"/>
+      <c r="I32" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
@@ -2801,7 +2859,9 @@
       <c r="H33" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I33" s="1"/>
+      <c r="I33" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
@@ -2843,7 +2903,9 @@
       <c r="H34" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I34" s="1"/>
+      <c r="I34" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
@@ -2885,7 +2947,9 @@
       <c r="H35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I35" s="1"/>
+      <c r="I35" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
@@ -2927,7 +2991,9 @@
       <c r="H36" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I36" s="1"/>
+      <c r="I36" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
@@ -2969,7 +3035,9 @@
       <c r="H37" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I37" s="1"/>
+      <c r="I37" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
@@ -3011,7 +3079,9 @@
       <c r="H38" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I38" s="1"/>
+      <c r="I38" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
@@ -3053,7 +3123,9 @@
       <c r="H39" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I39" s="1"/>
+      <c r="I39" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
@@ -3095,7 +3167,9 @@
       <c r="H40" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I40" s="1"/>
+      <c r="I40" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
@@ -3137,7 +3211,9 @@
       <c r="H41" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I41" s="1"/>
+      <c r="I41" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
@@ -3179,7 +3255,9 @@
       <c r="H42" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I42" s="1"/>
+      <c r="I42" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>

</xml_diff>